<commit_message>
Integrated graph coloring assignment
</commit_message>
<xml_diff>
--- a/div/status.xlsx
+++ b/div/status.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t xml:space="preserve">Problem</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t xml:space="preserve">10000_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next steps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why is DP for problems other than 30_0 NOT optimal? Is there a bug?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why does b&amp;b take so long? Should the evaluation change? Add best-first traversial to reduce time?</t>
   </si>
 </sst>
 </file>
@@ -130,6 +139,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -151,6 +161,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -158,6 +169,7 @@
       <color rgb="FF009900"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -302,17 +314,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:23"/>
+  <dimension ref="1:28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="26.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="26.1887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,6 +537,21 @@
       <c r="C23" s="3"/>
       <c r="D23" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>